<commit_message>
Made Druid, Cleric and Hunter for the new version.
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24030" windowHeight="12525"/>
+    <workbookView windowWidth="27630" windowHeight="12975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1013,8 +1013,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="41">
     <font>
@@ -1175,7 +1175,53 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1189,20 +1235,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1210,24 +1242,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1242,7 +1258,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1258,53 +1282,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1312,7 +1289,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1340,19 +1340,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1370,6 +1376,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1382,7 +1400,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1394,133 +1502,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1688,11 +1688,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1700,8 +1706,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1722,30 +1728,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1756,6 +1738,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1777,11 +1770,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1790,7 +1790,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1808,134 +1808,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="13" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2056,9 +2056,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2144,9 +2141,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2484,8 +2478,8 @@
   <sheetPr/>
   <dimension ref="A2:N148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2543,7 +2537,7 @@
       <c r="H5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="56" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2949,7 +2943,7 @@
       <c r="H19" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="I19" s="58" t="s">
+      <c r="I19" s="57" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3468,13 +3462,13 @@
       </c>
       <c r="F44" s="24"/>
       <c r="G44" s="25"/>
-      <c r="I44" s="56" t="s">
+      <c r="I44" s="55" t="s">
         <v>199</v>
       </c>
-      <c r="J44" s="49" t="s">
+      <c r="J44" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="K44" s="56"/>
+      <c r="K44" s="55"/>
     </row>
     <row r="45" ht="15.75" spans="2:11">
       <c r="B45" s="26" t="s">
@@ -3495,13 +3489,13 @@
       <c r="G45" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="I45" s="56" t="s">
+      <c r="I45" s="55" t="s">
         <v>201</v>
       </c>
-      <c r="J45" s="49" t="s">
+      <c r="J45" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="K45" s="56"/>
+      <c r="K45" s="55"/>
     </row>
     <row r="46" ht="15.75" spans="2:11">
       <c r="B46" s="30" t="s">
@@ -3522,13 +3516,13 @@
       <c r="G46" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="I46" s="56" t="s">
+      <c r="I46" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="J46" s="49" t="s">
+      <c r="J46" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="K46" s="49"/>
+      <c r="K46" s="48"/>
     </row>
     <row r="47" ht="16.5" spans="2:11">
       <c r="B47" s="32" t="s">
@@ -3547,13 +3541,13 @@
       <c r="G47" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="I47" s="56" t="s">
+      <c r="I47" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="J47" s="49" t="s">
+      <c r="J47" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="K47" s="49"/>
+      <c r="K47" s="48"/>
     </row>
     <row r="48" ht="16.5" spans="5:11">
       <c r="E48" s="32" t="s">
@@ -3565,20 +3559,20 @@
       <c r="G48" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="I48" s="59" t="s">
+      <c r="I48" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="J48" s="49" t="s">
+      <c r="J48" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="K48" s="49"/>
+      <c r="K48" s="48"/>
     </row>
     <row r="49" ht="15.75" spans="9:11">
-      <c r="I49" s="59" t="s">
+      <c r="I49" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="J49" s="59"/>
-      <c r="K49" s="56"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="55"/>
     </row>
     <row r="56" ht="15.75" spans="2:6">
       <c r="B56" s="2"/>
@@ -3602,31 +3596,31 @@
       <c r="E57" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="F57" s="40" t="s">
+      <c r="F57" s="39" t="s">
         <v>217</v>
       </c>
       <c r="G57" s="2"/>
-      <c r="H57" s="41" t="s">
+      <c r="H57" s="40" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="58" ht="15.75" spans="1:8">
-      <c r="A58" s="42">
+      <c r="A58" s="41">
         <v>0</v>
       </c>
-      <c r="B58" s="43">
+      <c r="B58" s="42">
         <v>0</v>
       </c>
       <c r="C58" s="2">
         <v>0</v>
       </c>
-      <c r="D58" s="44">
+      <c r="D58" s="43">
         <v>0</v>
       </c>
-      <c r="E58" s="45">
+      <c r="E58" s="44">
         <v>0</v>
       </c>
-      <c r="F58" s="46">
+      <c r="F58" s="45">
         <v>0</v>
       </c>
       <c r="G58" s="2"/>
@@ -3635,149 +3629,149 @@
       </c>
     </row>
     <row r="59" ht="15.75" spans="1:11">
-      <c r="A59" s="42">
+      <c r="A59" s="41">
         <v>0.5</v>
       </c>
-      <c r="B59" s="43">
+      <c r="B59" s="42">
         <v>0</v>
       </c>
-      <c r="C59" s="47">
+      <c r="C59" s="46">
         <v>8.5</v>
       </c>
-      <c r="D59" s="48">
+      <c r="D59" s="47">
         <v>4</v>
       </c>
-      <c r="E59" s="45">
+      <c r="E59" s="44">
         <v>0</v>
       </c>
-      <c r="F59" s="46">
+      <c r="F59" s="45">
         <v>5.5</v>
       </c>
       <c r="G59" s="2"/>
-      <c r="H59" s="47" t="s">
+      <c r="H59" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="K59" s="56"/>
+      <c r="K59" s="55"/>
     </row>
     <row r="60" ht="15.75" spans="1:11">
-      <c r="A60" s="42">
+      <c r="A60" s="41">
         <v>1</v>
       </c>
-      <c r="B60" s="43">
+      <c r="B60" s="42">
         <v>0</v>
       </c>
-      <c r="C60" s="49">
+      <c r="C60" s="48">
         <v>13</v>
       </c>
-      <c r="D60" s="48">
+      <c r="D60" s="47">
         <v>8</v>
       </c>
-      <c r="E60" s="45">
+      <c r="E60" s="44">
         <v>0</v>
       </c>
-      <c r="F60" s="46">
+      <c r="F60" s="45">
         <v>11</v>
       </c>
       <c r="G60" s="2"/>
-      <c r="H60" s="49" t="s">
+      <c r="H60" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="K60" s="56"/>
+      <c r="K60" s="55"/>
     </row>
     <row r="61" ht="15.75" spans="1:11">
-      <c r="A61" s="42">
+      <c r="A61" s="41">
         <v>0</v>
       </c>
-      <c r="B61" s="43">
+      <c r="B61" s="42">
         <v>1</v>
       </c>
-      <c r="C61" s="47">
+      <c r="C61" s="46">
         <v>8.5</v>
       </c>
-      <c r="D61" s="48">
+      <c r="D61" s="47">
         <v>4</v>
       </c>
-      <c r="E61" s="45">
+      <c r="E61" s="44">
         <v>4</v>
       </c>
-      <c r="F61" s="46">
+      <c r="F61" s="45">
         <v>5.5</v>
       </c>
       <c r="G61" s="2"/>
-      <c r="H61" s="47" t="s">
+      <c r="H61" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="K61" s="56"/>
+      <c r="K61" s="55"/>
     </row>
     <row r="62" ht="15.75" spans="1:11">
-      <c r="A62" s="42">
+      <c r="A62" s="41">
         <v>0.5</v>
       </c>
-      <c r="B62" s="43">
+      <c r="B62" s="42">
         <v>1</v>
       </c>
-      <c r="C62" s="49">
+      <c r="C62" s="48">
         <v>13</v>
       </c>
-      <c r="D62" s="48">
+      <c r="D62" s="47">
         <v>8</v>
       </c>
-      <c r="E62" s="45">
+      <c r="E62" s="44">
         <v>6</v>
       </c>
-      <c r="F62" s="46">
+      <c r="F62" s="45">
         <v>11</v>
       </c>
       <c r="G62" s="2"/>
-      <c r="H62" s="49" t="s">
+      <c r="H62" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="K62" s="56"/>
+      <c r="K62" s="55"/>
     </row>
     <row r="63" ht="16.5" spans="1:11">
-      <c r="A63" s="50">
+      <c r="A63" s="49">
         <v>1</v>
       </c>
-      <c r="B63" s="51">
+      <c r="B63" s="50">
         <v>1</v>
       </c>
-      <c r="C63" s="52">
+      <c r="C63" s="51">
         <v>17</v>
       </c>
-      <c r="D63" s="51">
+      <c r="D63" s="50">
         <v>12</v>
       </c>
-      <c r="E63" s="53">
+      <c r="E63" s="52">
         <v>8</v>
       </c>
-      <c r="F63" s="54">
+      <c r="F63" s="53">
         <v>16.5</v>
       </c>
       <c r="G63" s="2"/>
-      <c r="H63" s="49" t="s">
+      <c r="H63" s="48" t="s">
         <v>221</v>
       </c>
-      <c r="K63" s="56"/>
+      <c r="K63" s="55"/>
     </row>
     <row r="64" ht="15.75" spans="1:11">
-      <c r="A64" s="55"/>
-      <c r="B64" s="49"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="49"/>
+      <c r="A64" s="54"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="48"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="H64" s="56"/>
-      <c r="I64" s="56"/>
-      <c r="J64" s="56"/>
-      <c r="K64" s="56"/>
+      <c r="H64" s="55"/>
+      <c r="I64" s="55"/>
+      <c r="J64" s="55"/>
+      <c r="K64" s="55"/>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
-      <c r="C65" s="60" t="s">
+      <c r="C65" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="D65" s="60"/>
+      <c r="D65" s="59"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -3787,24 +3781,24 @@
       <c r="K65" s="2"/>
     </row>
     <row r="66" ht="15.75" spans="1:12">
-      <c r="A66" s="61" t="s">
+      <c r="A66" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="B66" s="62" t="s">
+      <c r="B66" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="C66" s="63" t="s">
+      <c r="C66" s="62" t="s">
         <v>223</v>
       </c>
-      <c r="D66" s="63"/>
-      <c r="E66" s="63"/>
-      <c r="F66" s="63"/>
-      <c r="G66" s="63"/>
-      <c r="H66" s="63"/>
-      <c r="I66" s="63"/>
-      <c r="J66" s="63"/>
-      <c r="K66" s="63"/>
-      <c r="L66" s="63"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="62"/>
+      <c r="F66" s="62"/>
+      <c r="G66" s="62"/>
+      <c r="H66" s="62"/>
+      <c r="I66" s="62"/>
+      <c r="J66" s="62"/>
+      <c r="K66" s="62"/>
+      <c r="L66" s="62"/>
     </row>
     <row r="67" spans="1:11">
       <c r="A67" s="2">
@@ -3813,10 +3807,10 @@
       <c r="B67" s="2">
         <v>0</v>
       </c>
-      <c r="C67" s="64" t="s">
+      <c r="C67" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="D67" s="64"/>
+      <c r="D67" s="63"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -3832,10 +3826,10 @@
       <c r="B68" s="2">
         <v>0</v>
       </c>
-      <c r="C68" s="64" t="s">
+      <c r="C68" s="63" t="s">
         <v>225</v>
       </c>
-      <c r="D68" s="64"/>
+      <c r="D68" s="63"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -3851,20 +3845,20 @@
       <c r="B69" s="2">
         <v>0</v>
       </c>
-      <c r="C69" s="64" t="s">
+      <c r="C69" s="63" t="s">
         <v>226</v>
       </c>
-      <c r="D69" s="64" t="s">
+      <c r="D69" s="63" t="s">
         <v>227</v>
       </c>
-      <c r="E69" s="64" t="s">
+      <c r="E69" s="63" t="s">
         <v>228</v>
       </c>
-      <c r="F69" s="65" t="s">
+      <c r="F69" s="64" t="s">
         <v>229</v>
       </c>
-      <c r="H69" s="64"/>
-      <c r="J69" s="65"/>
+      <c r="H69" s="63"/>
+      <c r="J69" s="64"/>
       <c r="K69" s="2"/>
     </row>
     <row r="70" spans="1:10">
@@ -3967,310 +3961,310 @@
       <c r="N73" s="2"/>
     </row>
     <row r="74" ht="15.75" spans="1:11">
-      <c r="A74" s="49"/>
-      <c r="B74" s="49"/>
-      <c r="C74" s="49"/>
-      <c r="D74" s="49"/>
-      <c r="E74" s="49"/>
-      <c r="F74" s="49"/>
-      <c r="G74" s="49"/>
-      <c r="H74" s="49"/>
+      <c r="A74" s="48"/>
+      <c r="B74" s="48"/>
+      <c r="C74" s="48"/>
+      <c r="D74" s="48"/>
+      <c r="E74" s="48"/>
+      <c r="F74" s="48"/>
+      <c r="G74" s="48"/>
+      <c r="H74" s="48"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
-      <c r="K74" s="49"/>
+      <c r="K74" s="48"/>
     </row>
     <row r="75" ht="15.75" spans="1:11">
-      <c r="A75" s="49"/>
-      <c r="B75" s="49" t="s">
+      <c r="A75" s="48"/>
+      <c r="B75" s="48" t="s">
         <v>245</v>
       </c>
-      <c r="C75" s="49"/>
-      <c r="D75" s="49"/>
-      <c r="E75" s="49" t="s">
+      <c r="C75" s="48"/>
+      <c r="D75" s="48"/>
+      <c r="E75" s="48" t="s">
         <v>246</v>
       </c>
-      <c r="F75" s="49"/>
-      <c r="G75" s="49"/>
-      <c r="H75" s="49"/>
+      <c r="F75" s="48"/>
+      <c r="G75" s="48"/>
+      <c r="H75" s="48"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
-      <c r="K75" s="49"/>
+      <c r="K75" s="48"/>
     </row>
     <row r="76" ht="15.75" spans="1:11">
-      <c r="A76" s="61"/>
-      <c r="B76" s="62" t="s">
+      <c r="A76" s="60"/>
+      <c r="B76" s="61" t="s">
         <v>247</v>
       </c>
       <c r="C76" s="3">
         <v>19</v>
       </c>
-      <c r="D76" s="66">
+      <c r="D76" s="65">
         <v>5</v>
       </c>
-      <c r="E76" s="62" t="s">
+      <c r="E76" s="61" t="s">
         <v>247</v>
       </c>
-      <c r="F76" s="67">
+      <c r="F76" s="66">
         <v>20</v>
       </c>
-      <c r="G76" s="66">
+      <c r="G76" s="65">
         <v>5</v>
       </c>
-      <c r="H76" s="66"/>
-      <c r="I76" s="66"/>
-      <c r="J76" s="66"/>
-      <c r="K76" s="66"/>
+      <c r="H76" s="65"/>
+      <c r="I76" s="65"/>
+      <c r="J76" s="65"/>
+      <c r="K76" s="65"/>
     </row>
     <row r="77" ht="15.75" spans="1:11">
-      <c r="A77" s="49"/>
-      <c r="B77" s="49" t="s">
+      <c r="A77" s="48"/>
+      <c r="B77" s="48" t="s">
         <v>248</v>
       </c>
-      <c r="C77" s="49">
+      <c r="C77" s="48">
         <v>10</v>
       </c>
-      <c r="D77" s="72" t="s">
+      <c r="D77" s="70" t="s">
         <v>249</v>
       </c>
-      <c r="E77" s="49" t="s">
+      <c r="E77" s="48" t="s">
         <v>248</v>
       </c>
-      <c r="F77" s="49">
+      <c r="F77" s="48">
         <v>4</v>
       </c>
-      <c r="G77" s="72" t="s">
+      <c r="G77" s="70" t="s">
         <v>249</v>
       </c>
-      <c r="H77" s="49"/>
+      <c r="H77" s="48"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
-      <c r="K77" s="49"/>
+      <c r="K77" s="48"/>
     </row>
     <row r="78" ht="15.75" spans="1:11">
-      <c r="A78" s="49"/>
-      <c r="B78" s="49" t="s">
+      <c r="A78" s="48"/>
+      <c r="B78" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="C78" s="49" t="s">
+      <c r="C78" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="D78" s="49" t="s">
+      <c r="D78" s="48" t="s">
         <v>252</v>
       </c>
-      <c r="E78" s="49" t="s">
+      <c r="E78" s="48" t="s">
         <v>253</v>
       </c>
-      <c r="F78" s="49">
+      <c r="F78" s="48">
         <v>10</v>
       </c>
-      <c r="G78" s="49"/>
-      <c r="H78" s="49"/>
+      <c r="G78" s="48"/>
+      <c r="H78" s="48"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
-      <c r="K78" s="49"/>
+      <c r="K78" s="48"/>
     </row>
     <row r="79" ht="15.75" spans="1:11">
-      <c r="A79" s="49"/>
-      <c r="B79" s="49" t="s">
+      <c r="A79" s="48"/>
+      <c r="B79" s="48" t="s">
         <v>254</v>
       </c>
-      <c r="C79" s="49">
+      <c r="C79" s="48">
         <v>12</v>
       </c>
-      <c r="D79" s="49"/>
-      <c r="E79" s="49" t="s">
+      <c r="D79" s="48"/>
+      <c r="E79" s="48" t="s">
         <v>254</v>
       </c>
-      <c r="F79" s="49">
+      <c r="F79" s="48">
         <v>12</v>
       </c>
-      <c r="G79" s="49"/>
-      <c r="H79" s="49"/>
+      <c r="G79" s="48"/>
+      <c r="H79" s="48"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
-      <c r="K79" s="49"/>
+      <c r="K79" s="48"/>
     </row>
     <row r="80" ht="15.75" spans="1:11">
-      <c r="A80" s="49"/>
-      <c r="B80" s="49"/>
-      <c r="C80" s="49"/>
-      <c r="D80" s="49"/>
-      <c r="E80" s="49"/>
-      <c r="F80" s="49"/>
-      <c r="G80" s="49"/>
-      <c r="H80" s="49"/>
+      <c r="A80" s="48"/>
+      <c r="B80" s="48"/>
+      <c r="C80" s="48"/>
+      <c r="D80" s="48"/>
+      <c r="E80" s="48"/>
+      <c r="F80" s="48"/>
+      <c r="G80" s="48"/>
+      <c r="H80" s="48"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
-      <c r="K80" s="49"/>
+      <c r="K80" s="48"/>
     </row>
     <row r="81" ht="15.75" spans="1:11">
-      <c r="A81" s="49"/>
-      <c r="B81" s="49" t="s">
+      <c r="A81" s="48"/>
+      <c r="B81" s="48" t="s">
         <v>255</v>
       </c>
-      <c r="C81" s="49" t="s">
+      <c r="C81" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="D81" s="49"/>
-      <c r="E81" s="49"/>
-      <c r="F81" s="49"/>
-      <c r="G81" s="49"/>
-      <c r="H81" s="49"/>
+      <c r="D81" s="48"/>
+      <c r="E81" s="48"/>
+      <c r="F81" s="48"/>
+      <c r="G81" s="48"/>
+      <c r="H81" s="48"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
-      <c r="K81" s="49"/>
+      <c r="K81" s="48"/>
     </row>
     <row r="82" ht="15.75" spans="1:11">
-      <c r="A82" s="49"/>
-      <c r="B82" s="49" t="s">
+      <c r="A82" s="48"/>
+      <c r="B82" s="48" t="s">
         <v>256</v>
       </c>
-      <c r="C82" s="49" t="s">
+      <c r="C82" s="48" t="s">
         <v>257</v>
       </c>
-      <c r="D82" s="49"/>
-      <c r="E82" s="49"/>
-      <c r="F82" s="49" t="s">
+      <c r="D82" s="48"/>
+      <c r="E82" s="48"/>
+      <c r="F82" s="48" t="s">
         <v>258</v>
       </c>
-      <c r="G82" s="49"/>
-      <c r="H82" s="49"/>
+      <c r="G82" s="48"/>
+      <c r="H82" s="48"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
-      <c r="K82" s="49"/>
+      <c r="K82" s="48"/>
     </row>
     <row r="83" ht="15.75" spans="1:11">
-      <c r="A83" s="49"/>
-      <c r="B83" s="49" t="s">
+      <c r="A83" s="48"/>
+      <c r="B83" s="48" t="s">
         <v>259</v>
       </c>
-      <c r="C83" s="49" t="s">
+      <c r="C83" s="48" t="s">
         <v>260</v>
       </c>
-      <c r="D83" s="49"/>
-      <c r="E83" s="49"/>
-      <c r="F83" s="49" t="s">
+      <c r="D83" s="48"/>
+      <c r="E83" s="48"/>
+      <c r="F83" s="48" t="s">
         <v>261</v>
       </c>
-      <c r="G83" s="49"/>
+      <c r="G83" s="48"/>
       <c r="H83" s="2"/>
-      <c r="I83" s="70"/>
+      <c r="I83" s="2"/>
       <c r="J83" s="2"/>
-      <c r="K83" s="49"/>
+      <c r="K83" s="48"/>
     </row>
     <row r="84" ht="15.75" spans="1:11">
-      <c r="A84" s="49"/>
-      <c r="B84" s="49" t="s">
+      <c r="A84" s="48"/>
+      <c r="B84" s="48" t="s">
         <v>262</v>
       </c>
-      <c r="C84" s="49" t="s">
+      <c r="C84" s="48" t="s">
         <v>263</v>
       </c>
-      <c r="D84" s="49"/>
-      <c r="E84" s="49"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="49"/>
+      <c r="D84" s="48"/>
+      <c r="E84" s="48"/>
+      <c r="F84" s="48"/>
+      <c r="G84" s="48"/>
       <c r="H84" s="2"/>
-      <c r="I84" s="70"/>
+      <c r="I84" s="2"/>
       <c r="J84" s="2"/>
-      <c r="K84" s="49"/>
+      <c r="K84" s="48"/>
     </row>
     <row r="85" ht="15.75" spans="1:11">
-      <c r="A85" s="49"/>
-      <c r="B85" s="49" t="s">
+      <c r="A85" s="48"/>
+      <c r="B85" s="48" t="s">
         <v>264</v>
       </c>
-      <c r="C85" s="49" t="s">
+      <c r="C85" s="48" t="s">
         <v>265</v>
       </c>
-      <c r="D85" s="49"/>
-      <c r="E85" s="49"/>
-      <c r="F85" s="49"/>
-      <c r="G85" s="49"/>
+      <c r="D85" s="48"/>
+      <c r="E85" s="48"/>
+      <c r="F85" s="48"/>
+      <c r="G85" s="48"/>
       <c r="H85" s="2"/>
-      <c r="I85" s="70"/>
+      <c r="I85" s="2"/>
       <c r="J85" s="2"/>
-      <c r="K85" s="49"/>
+      <c r="K85" s="48"/>
     </row>
     <row r="86" ht="15.75" spans="1:11">
-      <c r="A86" s="49"/>
-      <c r="B86" s="49" t="s">
+      <c r="A86" s="48"/>
+      <c r="B86" s="48" t="s">
         <v>266</v>
       </c>
-      <c r="C86" s="49" t="s">
+      <c r="C86" s="48" t="s">
         <v>267</v>
       </c>
-      <c r="D86" s="49"/>
-      <c r="E86" s="49"/>
-      <c r="F86" s="49"/>
-      <c r="G86" s="49"/>
+      <c r="D86" s="48"/>
+      <c r="E86" s="48"/>
+      <c r="F86" s="48"/>
+      <c r="G86" s="48"/>
       <c r="H86" s="2"/>
-      <c r="I86" s="70"/>
+      <c r="I86" s="2"/>
       <c r="J86" s="2"/>
-      <c r="K86" s="49"/>
+      <c r="K86" s="48"/>
     </row>
     <row r="87" ht="15.75" spans="1:11">
-      <c r="A87" s="49"/>
-      <c r="B87" s="49"/>
-      <c r="C87" s="49"/>
-      <c r="D87" s="49"/>
-      <c r="E87" s="49"/>
-      <c r="F87" s="49"/>
-      <c r="G87" s="49"/>
-      <c r="H87" s="49"/>
+      <c r="A87" s="48"/>
+      <c r="B87" s="48"/>
+      <c r="C87" s="48"/>
+      <c r="D87" s="48"/>
+      <c r="E87" s="48"/>
+      <c r="F87" s="48"/>
+      <c r="G87" s="48"/>
+      <c r="H87" s="48"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
-      <c r="K87" s="49"/>
+      <c r="K87" s="48"/>
     </row>
     <row r="88" ht="15.75" spans="1:13">
-      <c r="A88" s="56"/>
-      <c r="B88" s="56"/>
-      <c r="C88" s="56"/>
-      <c r="D88" s="56"/>
-      <c r="E88" s="56"/>
-      <c r="F88" s="56"/>
-      <c r="G88" s="56"/>
-      <c r="H88" s="56"/>
-      <c r="I88" s="56"/>
-      <c r="J88" s="56"/>
-      <c r="K88" s="56"/>
-      <c r="M88" s="49"/>
+      <c r="A88" s="55"/>
+      <c r="B88" s="55"/>
+      <c r="C88" s="55"/>
+      <c r="D88" s="55"/>
+      <c r="E88" s="55"/>
+      <c r="F88" s="55"/>
+      <c r="G88" s="55"/>
+      <c r="H88" s="55"/>
+      <c r="I88" s="55"/>
+      <c r="J88" s="55"/>
+      <c r="K88" s="55"/>
+      <c r="M88" s="48"/>
     </row>
     <row r="89" ht="15.75" spans="1:13">
-      <c r="A89" s="56"/>
-      <c r="B89" s="56"/>
-      <c r="C89" s="49" t="s">
+      <c r="A89" s="55"/>
+      <c r="B89" s="55"/>
+      <c r="C89" s="48" t="s">
         <v>268</v>
       </c>
-      <c r="D89" s="49"/>
-      <c r="E89" s="56"/>
-      <c r="F89" s="56"/>
-      <c r="G89" s="56"/>
-      <c r="H89" s="56"/>
-      <c r="I89" s="56"/>
-      <c r="J89" s="56"/>
-      <c r="K89" s="56"/>
-      <c r="M89" s="49"/>
+      <c r="D89" s="48"/>
+      <c r="E89" s="55"/>
+      <c r="F89" s="55"/>
+      <c r="G89" s="55"/>
+      <c r="H89" s="55"/>
+      <c r="I89" s="55"/>
+      <c r="J89" s="55"/>
+      <c r="K89" s="55"/>
+      <c r="M89" s="48"/>
     </row>
     <row r="90" ht="15.75" spans="1:13">
-      <c r="A90" s="61" t="s">
+      <c r="A90" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="B90" s="62" t="s">
+      <c r="B90" s="61" t="s">
         <v>213</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>269</v>
       </c>
       <c r="D90" s="3"/>
-      <c r="E90" s="49"/>
-      <c r="F90" s="49"/>
-      <c r="G90" s="49"/>
-      <c r="H90" s="49"/>
-      <c r="I90" s="49"/>
-      <c r="J90" s="49"/>
-      <c r="K90" s="49"/>
-      <c r="M90" s="49"/>
+      <c r="E90" s="48"/>
+      <c r="F90" s="48"/>
+      <c r="G90" s="48"/>
+      <c r="H90" s="48"/>
+      <c r="I90" s="48"/>
+      <c r="J90" s="48"/>
+      <c r="K90" s="48"/>
+      <c r="M90" s="48"/>
     </row>
     <row r="91" spans="1:11">
       <c r="A91" s="2">
@@ -4355,10 +4349,10 @@
     <row r="95" spans="1:11">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
-      <c r="C95" s="60" t="s">
+      <c r="C95" s="59" t="s">
         <v>222</v>
       </c>
-      <c r="D95" s="60"/>
+      <c r="D95" s="59"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -4368,24 +4362,24 @@
       <c r="K95" s="2"/>
     </row>
     <row r="96" ht="15.75" spans="1:12">
-      <c r="A96" s="61" t="s">
+      <c r="A96" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="B96" s="62" t="s">
+      <c r="B96" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="C96" s="63" t="s">
+      <c r="C96" s="62" t="s">
         <v>223</v>
       </c>
-      <c r="D96" s="63"/>
-      <c r="E96" s="63"/>
-      <c r="F96" s="63"/>
-      <c r="G96" s="63"/>
-      <c r="H96" s="63"/>
-      <c r="I96" s="63"/>
-      <c r="J96" s="63"/>
-      <c r="K96" s="63"/>
-      <c r="L96" s="63"/>
+      <c r="D96" s="62"/>
+      <c r="E96" s="62"/>
+      <c r="F96" s="62"/>
+      <c r="G96" s="62"/>
+      <c r="H96" s="62"/>
+      <c r="I96" s="62"/>
+      <c r="J96" s="62"/>
+      <c r="K96" s="62"/>
+      <c r="L96" s="62"/>
     </row>
     <row r="97" spans="1:11">
       <c r="A97" s="2">
@@ -4394,10 +4388,10 @@
       <c r="B97" s="2">
         <v>0</v>
       </c>
-      <c r="C97" s="64" t="s">
+      <c r="C97" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="D97" s="64"/>
+      <c r="D97" s="63"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -4413,10 +4407,10 @@
       <c r="B98" s="2">
         <v>0</v>
       </c>
-      <c r="C98" s="64" t="s">
+      <c r="C98" s="63" t="s">
         <v>225</v>
       </c>
-      <c r="D98" s="64"/>
+      <c r="D98" s="63"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -4432,22 +4426,22 @@
       <c r="B99" s="2">
         <v>0</v>
       </c>
-      <c r="C99" s="64" t="s">
+      <c r="C99" s="63" t="s">
         <v>226</v>
       </c>
-      <c r="D99" s="64"/>
-      <c r="E99" s="64" t="s">
+      <c r="D99" s="63"/>
+      <c r="E99" s="63" t="s">
         <v>227</v>
       </c>
-      <c r="F99" s="64"/>
-      <c r="G99" s="64" t="s">
+      <c r="F99" s="63"/>
+      <c r="G99" s="63" t="s">
         <v>228</v>
       </c>
-      <c r="H99" s="64"/>
-      <c r="I99" s="65" t="s">
+      <c r="H99" s="63"/>
+      <c r="I99" s="64" t="s">
         <v>224</v>
       </c>
-      <c r="J99" s="65"/>
+      <c r="J99" s="64"/>
       <c r="K99" s="2"/>
     </row>
     <row r="100" spans="1:11">
@@ -4670,24 +4664,24 @@
       <c r="N108" s="2"/>
     </row>
     <row r="109" ht="15.75" spans="1:14">
-      <c r="A109" s="61" t="s">
+      <c r="A109" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="B109" s="62" t="s">
+      <c r="B109" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="C109" s="68" t="s">
+      <c r="C109" s="67" t="s">
         <v>273</v>
       </c>
-      <c r="D109" s="68"/>
-      <c r="E109" s="69" t="s">
+      <c r="D109" s="67"/>
+      <c r="E109" s="68" t="s">
         <v>274</v>
       </c>
-      <c r="F109" s="69"/>
-      <c r="G109" s="64" t="s">
+      <c r="F109" s="68"/>
+      <c r="G109" s="63" t="s">
         <v>275</v>
       </c>
-      <c r="H109" s="64"/>
+      <c r="H109" s="63"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
@@ -5220,10 +5214,10 @@
         <v>211</v>
       </c>
       <c r="D135" s="2"/>
-      <c r="E135" s="71" t="s">
+      <c r="E135" s="69" t="s">
         <v>296</v>
       </c>
-      <c r="F135" s="71"/>
+      <c r="F135" s="69"/>
     </row>
     <row r="136" spans="3:7">
       <c r="C136" s="2" t="s">

</xml_diff>